<commit_message>
added Paged List, timelog
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D52067-BA92-4B47-8583-F64F0CA9F812}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFA74DC-3FBF-4EE9-872A-48F240C6340A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3996" yWindow="2556" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
     <sheet name="Nädal 2" sheetId="2" r:id="rId2"/>
     <sheet name="Nädal 3" sheetId="3" r:id="rId3"/>
     <sheet name="Nädal 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="60">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>delegate, lambda</t>
+  </si>
+  <si>
+    <t>vead</t>
+  </si>
+  <si>
+    <t>vigade parandus</t>
+  </si>
+  <si>
+    <t>W6 loeng</t>
+  </si>
+  <si>
+    <t>HW5, video 7 lõpuni</t>
   </si>
 </sst>
 </file>
@@ -2699,7 +2711,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2916,14 +2928,18 @@
       <c r="C9" s="8">
         <v>0.875</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.9375</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>90</v>
+      </c>
       <c r="G9" s="6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -2932,13 +2948,25 @@
       <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="7">
+        <v>43893</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="F10" s="5">
+        <v>90</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -2946,14 +2974,28 @@
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="7">
+        <v>43893</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="F11" s="5">
+        <v>50</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -3036,7 +3078,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>350</v>
+        <v>580</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
added SustemOfUnitData, UnitData, UnitFactorData, migrations
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFA74DC-3FBF-4EE9-872A-48F240C6340A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8521294-1F1E-4332-B723-3B3E20798076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4344" yWindow="2904" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="61">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>HW5, video 7 lõpuni</t>
+  </si>
+  <si>
+    <t>HW5, video 8, 9</t>
   </si>
 </sst>
 </file>
@@ -2974,9 +2977,7 @@
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
-        <v>43893</v>
-      </c>
+      <c r="B11" s="7"/>
       <c r="C11" s="8">
         <v>0.77777777777777779</v>
       </c>
@@ -3003,12 +3004,18 @@
         <v>9</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>

</xml_diff>

<commit_message>
Added 4 tests and timelog update
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8521294-1F1E-4332-B723-3B3E20798076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A15788-AB5F-42EC-AA7F-EDA15E398076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4344" yWindow="2904" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2714,7 +2714,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3007,16 +3007,24 @@
       <c r="C12" s="8">
         <v>0.92708333333333337</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5">
+        <v>85</v>
+      </c>
       <c r="G12" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -3085,7 +3093,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>580</v>
+        <v>665</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
total of 12 tests passed, 3 tests in 4 classes
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C22B1A-0513-4543-8F97-F3CABF2A2ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCDB0B6-4641-4593-8D6E-F2F4029829E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4344" yWindow="2904" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2717,7 +2717,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3040,9 +3040,13 @@
       <c r="C13" s="8">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>0.9375</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>60</v>
+      </c>
       <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
@@ -3104,7 +3108,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>665</v>
+        <v>725</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
20 tests passed, corrected bugs
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCDB0B6-4641-4593-8D6E-F2F4029829E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C241E4A-0DDD-4EA0-AB70-87D76088CDB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4344" yWindow="2904" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="64">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>HW5, video 10</t>
+  </si>
+  <si>
+    <t>prakt.</t>
+  </si>
+  <si>
+    <t>kodutöö kaitmine, täiendamine</t>
   </si>
 </sst>
 </file>
@@ -2716,7 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFEB4F-7E20-42AE-B220-1C3E7DAEF925}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -2725,7 +2731,7 @@
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3054,19 +3060,29 @@
         <v>61</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="10"/>
+      <c r="J13" s="10">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7">
+        <v>43895</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>

</xml_diff>

<commit_message>
added Aids, 30 tests passed
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7F4AEB-DA93-46B6-8084-DE2422990778}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2939A6D9-60C7-45C8-92B6-8CE52C9D1DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4344" yWindow="2904" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="65">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -228,7 +228,10 @@
     <t>prakt.</t>
   </si>
   <si>
-    <t>kodutöö kaitsmine, täiendamine</t>
+    <t>kodutöö kaitsmine, täiendamine, v10</t>
+  </si>
+  <si>
+    <t>V11</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1887,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:J19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2261,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ED01CA-374D-44E5-ADBC-2090FD744E32}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2722,8 +2725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFEB4F-7E20-42AE-B220-1C3E7DAEF925}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3074,16 +3077,22 @@
       <c r="C14" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <v>0.48958333333333331</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>195</v>
+      </c>
       <c r="G14" s="6" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -3091,12 +3100,22 @@
         <v>12</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="8">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.99305555555555547</v>
+      </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="F15" s="5">
+        <v>90</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -3124,7 +3143,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>725</v>
+        <v>1010</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
TimeLog, video 12 done, 30 tests passed
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C9AE7-ED88-45D5-83BE-01DEB2A6C172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D024216-8370-41C4-9755-B71DE500BF50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="67">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>V11</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>V13</t>
   </si>
 </sst>
 </file>
@@ -3192,7 +3198,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3275,27 +3281,45 @@
       <c r="C4" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
+      <c r="D4" s="19">
+        <v>0.625</v>
+      </c>
+      <c r="E4" s="20">
+        <v>15</v>
+      </c>
+      <c r="F4" s="21">
+        <v>105</v>
+      </c>
       <c r="G4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="H4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="7">
+        <v>43899</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.6875</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="6"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="G5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -3462,7 +3486,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -3471,12 +3495,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V15, Created _CRUD layouts
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D024216-8370-41C4-9755-B71DE500BF50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE2117-5043-4338-8950-C7ABF0321CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="68">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -238,7 +238,10 @@
     <t>V12</t>
   </si>
   <si>
-    <t>V13</t>
+    <t>V13, 14</t>
+  </si>
+  <si>
+    <t>V15</t>
   </si>
 </sst>
 </file>
@@ -3198,7 +3201,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3301,7 +3304,7 @@
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3311,32 +3314,53 @@
       <c r="C5" s="8">
         <v>0.6875</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
+      <c r="D5" s="8">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E5" s="6">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5">
+        <v>215</v>
+      </c>
       <c r="G5" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>66</v>
       </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="F6" s="5">
+        <v>50</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3345,12 +3369,14 @@
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3359,12 +3385,14 @@
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3373,12 +3401,14 @@
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3387,12 +3417,14 @@
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3401,12 +3433,14 @@
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3415,12 +3449,14 @@
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3429,12 +3465,14 @@
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3443,12 +3481,14 @@
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3457,7 +3497,9 @@
       <c r="D15" s="8"/>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -3471,7 +3513,9 @@
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="26"/>
+      <c r="G16" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="26"/>
       <c r="J16" s="27"/>
@@ -3486,7 +3530,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>105</v>
+        <v>370</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V16, shortened CRUD html pages
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE2117-5043-4338-8950-C7ABF0321CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E107881-9B9B-43FB-8DF4-51840AF69A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3201,7 +3201,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3365,7 +3365,9 @@
         <v>4</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>

</xml_diff>

<commit_message>
V17, refactored user interface, sorting
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E107881-9B9B-43FB-8DF4-51840AF69A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9596F8FC-3723-4DF3-8CBA-46A46E53C923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="69">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>V15</t>
+  </si>
+  <si>
+    <t>V16, 17</t>
   </si>
 </sst>
 </file>
@@ -3201,7 +3204,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3368,14 +3371,24 @@
       <c r="C7" s="8">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5">
+        <v>120</v>
+      </c>
       <c r="G7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3532,7 +3545,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>370</v>
+        <v>490</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
Sorting regular and descending
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87ACEA18-0355-493F-84AB-F435C54D8529}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935E62CE-05FF-4E12-A18B-CEA5DCA0B2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="72">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>nädal7</t>
+  </si>
+  <si>
+    <t>V19</t>
   </si>
 </sst>
 </file>
@@ -3210,7 +3213,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3446,7 +3449,9 @@
       <c r="H9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3454,14 +3459,18 @@
         <v>7</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
       <c r="G10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>

</xml_diff>

<commit_message>
Created Tests for Sorted Repo
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935E62CE-05FF-4E12-A18B-CEA5DCA0B2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB0EB4D-45A5-4EA4-9C9C-EBD5DA096AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="73">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -253,7 +253,10 @@
     <t>nädal7</t>
   </si>
   <si>
-    <t>V19</t>
+    <t>V19, 20</t>
+  </si>
+  <si>
+    <t>V20</t>
   </si>
 </sst>
 </file>
@@ -3212,8 +3215,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3462,9 +3465,13 @@
       <c r="C10" s="8">
         <v>0.94791666666666663</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>45</v>
+      </c>
       <c r="G10" s="20" t="s">
         <v>27</v>
       </c>
@@ -3479,14 +3486,18 @@
         <v>8</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
       <c r="G11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -3580,7 +3591,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>655</v>
+        <v>700</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
Sorted 41 test are complete
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7576D957-05A8-4C31-8B44-8DA5F6D367CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADC365F-7F20-473F-B492-61FDCAE8290A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,7 @@
     <t>V20</t>
   </si>
   <si>
-    <t>V21</t>
+    <t>V21, 22</t>
   </si>
 </sst>
 </file>
@@ -3218,8 +3218,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3524,9 +3524,15 @@
       <c r="C12" s="8">
         <v>0.38541666666666669</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="8">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E12" s="6">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5">
+        <v>155</v>
+      </c>
       <c r="G12" s="20" t="s">
         <v>27</v>
       </c>
@@ -3610,7 +3616,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>840</v>
+        <v>995</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
Repository classes refactoring, just before removing PaginatedList
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADC365F-7F20-473F-B492-61FDCAE8290A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A3D1FF-3798-4F44-843C-C539C45D6379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="75">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -259,7 +259,10 @@
     <t>V20</t>
   </si>
   <si>
-    <t>V21, 22</t>
+    <t>V21, 22, 23</t>
+  </si>
+  <si>
+    <t>V24</t>
   </si>
 </sst>
 </file>
@@ -3219,7 +3222,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3539,7 +3542,9 @@
       <c r="H12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3547,14 +3552,18 @@
         <v>10</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
       <c r="G13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>

</xml_diff>

<commit_message>
Cleaned Code, remowed unused sentences, Cleaned up MeasureRepository, Video26 is done for 10 min.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A3D1FF-3798-4F44-843C-C539C45D6379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B87D788-8E8B-49CC-ABEF-EA265838E60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="76">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>V24</t>
+  </si>
+  <si>
+    <t>V25</t>
   </si>
 </sst>
 </file>
@@ -3222,7 +3225,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3555,16 +3558,22 @@
       <c r="C13" s="8">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>60</v>
+      </c>
       <c r="G13" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3572,16 +3581,26 @@
         <v>11</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="8">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>35</v>
+      </c>
       <c r="G14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="I14" s="6"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="10">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
@@ -3625,7 +3644,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>995</v>
+        <v>1090</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
Completed Filetred Repository refactoring
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B87D788-8E8B-49CC-ABEF-EA265838E60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA9A22A-8D8C-40B7-8D91-A66C6FB7FC44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Nädal 4" sheetId="4" r:id="rId4"/>
     <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
     <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="78">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -266,6 +267,12 @@
   </si>
   <si>
     <t>V25</t>
+  </si>
+  <si>
+    <t>vide</t>
+  </si>
+  <si>
+    <t>V27, 28</t>
   </si>
 </sst>
 </file>
@@ -3220,12 +3227,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E8D5A3-EE29-4B00-8CB8-84335370DF7E}">
   <sheetPr>
-    <tabColor rgb="FF92D050"/>
+    <tabColor rgb="FFFF7C80"/>
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3662,4 +3669,301 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE15974-5033-406C-AF67-B3DBF83F5800}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="43">
+        <v>43909</v>
+      </c>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
+    </row>
+    <row r="3" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18">
+        <v>43903</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="30">
+        <f>SUM(F4:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A17:E17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
V28 edasi, Timelog update, MeasureView taastatud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D58A5B2-86E8-4C19-A306-18B5B231C41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8A43A4-AC8E-4805-B865-53B753B11F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="78">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -269,7 +269,10 @@
     <t>V25</t>
   </si>
   <si>
-    <t>V27, 28</t>
+    <t>V27</t>
+  </si>
+  <si>
+    <t>V28</t>
   </si>
 </sst>
 </file>
@@ -3676,7 +3679,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3781,25 +3784,45 @@
         <v>2</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="8">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="J5" s="10"/>
+      <c r="F5" s="5">
+        <v>30</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" s="10">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="7">
+        <v>43905</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.59375</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="6"/>
+      <c r="G6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="10"/>
     </row>
@@ -3812,7 +3835,9 @@
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="10"/>
@@ -3826,7 +3851,9 @@
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
@@ -3840,7 +3867,9 @@
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -3854,7 +3883,9 @@
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -3953,7 +3984,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
timelog, Video28, Indexist kõik asjad viidus MeasurePage'i
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8A43A4-AC8E-4805-B865-53B753B11F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB6F946-AAAC-48D1-B115-E62DCC073603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1008" windowWidth="14916" windowHeight="8964" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3516" yWindow="1068" windowWidth="14916" windowHeight="8964" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="81">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>V28</t>
+  </si>
+  <si>
+    <t>V28,29</t>
+  </si>
+  <si>
+    <t>apps</t>
+  </si>
+  <si>
+    <t>trello, slack</t>
   </si>
 </sst>
 </file>
@@ -3679,12 +3688,13 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" customWidth="1"/>
     <col min="9" max="9" width="4.5546875" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
   </cols>
@@ -3814,14 +3824,18 @@
       <c r="C6" s="8">
         <v>0.59375</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5">
+        <v>75</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="10"/>
@@ -3830,16 +3844,28 @@
       <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="7">
+        <v>43909</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>30</v>
+      </c>
       <c r="G7" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3847,9 +3873,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6">
+        <v>10</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="20" t="s">
         <v>27</v>
@@ -3984,7 +4014,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
lisatud Units lehed, kopeeritud Measures lehtedelt
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB6F946-AAAC-48D1-B115-E62DCC073603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677D9C6A-02C4-4BC0-A336-0E1F753F1F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3516" yWindow="1068" windowWidth="14916" windowHeight="8964" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="6">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="20" t="s">

</xml_diff>

<commit_message>
75 testi kokku, 1 kukkus läbi, Video32 (1/3 tehtud)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677D9C6A-02C4-4BC0-A336-0E1F753F1F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1BC07E-725F-49DC-9A24-E5392913067F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3516" yWindow="1068" windowWidth="14916" windowHeight="8964" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="82">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>trello, slack</t>
+  </si>
+  <si>
+    <t>V30, 31, 32</t>
   </si>
 </sst>
 </file>
@@ -3688,7 +3691,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3876,17 +3879,25 @@
       <c r="C8" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8">
+        <v>0.96875</v>
+      </c>
       <c r="E8" s="6">
-        <v>40</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F8" s="5">
+        <v>375</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="10">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
@@ -4014,7 +4025,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>180</v>
+        <v>555</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
Video 32, 113 teste läksid läbi
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1BC07E-725F-49DC-9A24-E5392913067F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A05A57-1687-4BAD-A938-D98DC88C4431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3516" yWindow="1068" windowWidth="14916" windowHeight="8964" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
     <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
     <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="84">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -285,6 +286,12 @@
   </si>
   <si>
     <t>V30, 31, 32</t>
+  </si>
+  <si>
+    <t>20.03 - 26.03.2020</t>
+  </si>
+  <si>
+    <t>V32</t>
   </si>
 </sst>
 </file>
@@ -1074,21 +1081,21 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1109,7 @@
       <c r="I2" s="37"/>
       <c r="J2" s="38"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -1114,7 +1121,7 @@
       <c r="I3" s="40"/>
       <c r="J3" s="41"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>1</v>
       </c>
@@ -1134,7 +1141,7 @@
       <c r="I4" s="43"/>
       <c r="J4" s="44"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
@@ -1146,7 +1153,7 @@
       <c r="I5" s="46"/>
       <c r="J5" s="47"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>3</v>
       </c>
@@ -1176,7 +1183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1206,7 +1213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -1266,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -1294,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -1322,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -1364,7 +1371,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -1378,7 +1385,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -1392,7 +1399,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -1406,7 +1413,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -1420,7 +1427,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -1434,7 +1441,7 @@
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>12</v>
       </c>
@@ -1477,24 +1484,24 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="29.88671875" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" customWidth="1"/>
-    <col min="10" max="10" width="3.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
@@ -1508,7 +1515,7 @@
       <c r="I2" s="37"/>
       <c r="J2" s="38"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -1520,7 +1527,7 @@
       <c r="I3" s="40"/>
       <c r="J3" s="41"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>1</v>
       </c>
@@ -1540,7 +1547,7 @@
       <c r="I4" s="43"/>
       <c r="J4" s="44"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
@@ -1552,7 +1559,7 @@
       <c r="I5" s="46"/>
       <c r="J5" s="47"/>
     </row>
-    <row r="6" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1612,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -1639,7 +1646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -1667,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -1693,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -1719,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -1747,7 +1754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -1777,7 +1784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -1805,7 +1812,7 @@
       </c>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -1835,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -1861,7 +1868,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -1887,7 +1894,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -1915,7 +1922,7 @@
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>12</v>
       </c>
@@ -1957,22 +1964,22 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
@@ -1986,7 +1993,7 @@
       <c r="I2" s="37"/>
       <c r="J2" s="38"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -1998,7 +2005,7 @@
       <c r="I3" s="40"/>
       <c r="J3" s="41"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>1</v>
       </c>
@@ -2018,7 +2025,7 @@
       <c r="I4" s="43"/>
       <c r="J4" s="44"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
@@ -2030,7 +2037,7 @@
       <c r="I5" s="46"/>
       <c r="J5" s="47"/>
     </row>
-    <row r="6" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>3</v>
       </c>
@@ -2060,7 +2067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -2086,7 +2093,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -2116,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -2144,7 +2151,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -2172,7 +2179,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -2198,7 +2205,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -2212,7 +2219,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -2226,7 +2233,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -2240,7 +2247,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -2254,7 +2261,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -2268,7 +2275,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -2282,7 +2289,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -2296,7 +2303,7 @@
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>12</v>
       </c>
@@ -2338,22 +2345,22 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
@@ -2367,7 +2374,7 @@
       <c r="I2" s="37"/>
       <c r="J2" s="38"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -2379,7 +2386,7 @@
       <c r="I3" s="40"/>
       <c r="J3" s="41"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>1</v>
       </c>
@@ -2399,7 +2406,7 @@
       <c r="I4" s="43"/>
       <c r="J4" s="44"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
@@ -2411,7 +2418,7 @@
       <c r="I5" s="46"/>
       <c r="J5" s="47"/>
     </row>
-    <row r="6" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>3</v>
       </c>
@@ -2441,7 +2448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -2467,7 +2474,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -2490,7 +2497,7 @@
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -2518,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -2546,7 +2553,7 @@
       </c>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -2576,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -2608,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -2634,7 +2641,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -2660,7 +2667,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -2690,7 +2697,7 @@
       </c>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -2718,7 +2725,7 @@
       </c>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -2732,7 +2739,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>12</v>
       </c>
@@ -2746,7 +2753,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>13</v>
       </c>
@@ -2760,7 +2767,7 @@
       <c r="I19" s="26"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
         <v>12</v>
       </c>
@@ -2802,15 +2809,15 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>1</v>
       </c>
@@ -2830,7 +2837,7 @@
       <c r="I1" s="43"/>
       <c r="J1" s="44"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -2842,7 +2849,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -2872,7 +2879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -2900,7 +2907,7 @@
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2928,7 +2935,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2954,7 +2961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2984,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3008,7 +3015,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3032,7 +3039,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3058,7 +3065,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3084,7 +3091,7 @@
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3112,7 +3119,7 @@
       </c>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3140,7 +3147,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3168,7 +3175,7 @@
       </c>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3192,7 +3199,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3206,7 +3213,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>12</v>
       </c>
@@ -3247,15 +3254,15 @@
       <selection sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" customWidth="1"/>
-    <col min="9" max="9" width="3.5546875" customWidth="1"/>
-    <col min="10" max="10" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.5703125" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>1</v>
       </c>
@@ -3275,7 +3282,7 @@
       <c r="I1" s="43"/>
       <c r="J1" s="44"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -3287,7 +3294,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -3317,7 +3324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -3347,7 +3354,7 @@
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3377,7 +3384,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -3403,7 +3410,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3431,7 +3438,7 @@
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3459,7 +3466,7 @@
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3485,7 +3492,7 @@
       </c>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3509,7 +3516,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3539,7 +3546,7 @@
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3569,7 +3576,7 @@
       </c>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3595,7 +3602,7 @@
       </c>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3621,7 +3628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3637,7 +3644,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3653,7 +3660,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>12</v>
       </c>
@@ -3686,23 +3693,23 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE15974-5033-406C-AF67-B3DBF83F5800}">
   <sheetPr>
-    <tabColor rgb="FF92D050"/>
+    <tabColor rgb="FFFF7C80"/>
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" customWidth="1"/>
-    <col min="9" max="9" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>1</v>
       </c>
@@ -3722,7 +3729,7 @@
       <c r="I1" s="43"/>
       <c r="J1" s="44"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -3734,7 +3741,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -3764,7 +3771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -3792,7 +3799,7 @@
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3817,7 +3824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -3843,7 +3850,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3871,7 +3878,7 @@
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3899,7 +3906,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3908,14 +3915,12 @@
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="G9" s="20"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3924,14 +3929,12 @@
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="G10" s="20"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3945,7 +3948,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3959,7 +3962,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3973,7 +3976,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3987,7 +3990,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -4001,7 +4004,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -4015,7 +4018,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>12</v>
       </c>
@@ -4043,4 +4046,332 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CA3D4A-EC4E-4EB5-A47F-751E9C58F477}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="10" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="44"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
+    </row>
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18">
+        <v>43910</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21">
+        <v>60</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="22">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>43911</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.59375</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5">
+        <v>75</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="30">
+        <f>SUM(F4:F16)</f>
+        <v>135</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A17:E17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Loeng 34 (Võõrvõtme sisu näitamine)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A0329-C3CA-4145-AC09-CF59A7F7BDCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F2966F-5425-49BF-96DE-728875763914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="85">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -4059,7 +4059,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4195,18 +4195,24 @@
       <c r="C6" s="8">
         <v>0.77777777777777779</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8">
+        <v>0.84722222222222221</v>
+      </c>
       <c r="E6" s="6">
         <v>15</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5">
+        <v>85</v>
+      </c>
       <c r="G6" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4214,9 +4220,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8">
+        <v>0.84722222222222221</v>
+      </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6">
+        <v>35</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="20" t="s">
         <v>27</v>
@@ -4365,7 +4375,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>135</v>
+        <v>220</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
Master-Details, video 36, Measures -> Show units page (peaaegu töötab)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02B71CF-64F8-459B-B734-A15147D25334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5080CA-787A-41CF-AADB-C1977B8C8EE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-570" yWindow="2070" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="87">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -298,6 +299,9 @@
   </si>
   <si>
     <t>V34</t>
+  </si>
+  <si>
+    <t>V35, 36</t>
   </si>
 </sst>
 </file>
@@ -4062,7 +4066,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4250,16 +4254,30 @@
       <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
+      <c r="B8" s="7">
+        <v>43913</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>55</v>
+      </c>
+      <c r="F8" s="5">
+        <v>230</v>
+      </c>
       <c r="G8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4386,7 +4404,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>335</v>
+        <v>565</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V37, Master Detail lõpuni tehtud,
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5080CA-787A-41CF-AADB-C1977B8C8EE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73947DA-4E28-4691-B8A5-9DD106D5F3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-570" yWindow="2070" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2070" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="88">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -301,7 +300,10 @@
     <t>V34</t>
   </si>
   <si>
-    <t>V35, 36</t>
+    <t>V35, 36, KT7 korras</t>
+  </si>
+  <si>
+    <t>V37</t>
   </si>
 </sst>
 </file>
@@ -4284,15 +4286,21 @@
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="7">
+        <v>43914</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
       <c r="G9" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>

</xml_diff>

<commit_message>
V38, master detail refaktoorimine, just enne testide tegemist
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73947DA-4E28-4691-B8A5-9DD106D5F3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C79E8E4-530F-49EE-8470-912FA0FBCBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2070" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="89">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>V37</t>
+  </si>
+  <si>
+    <t>V38</t>
   </si>
 </sst>
 </file>
@@ -4068,7 +4071,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4292,16 +4295,22 @@
       <c r="C9" s="8">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>90</v>
+      </c>
       <c r="G9" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4309,12 +4318,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8">
+        <v>0.875</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -4412,7 +4425,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>565</v>
+        <v>655</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V39, 181/197 teste läbitud. Üks test feilis - IsExtensionsTested. parandan pärast.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C79E8E4-530F-49EE-8470-912FA0FBCBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5C75F1-C874-4FD2-818B-961F7E05A1D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2070" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
     <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Nädal 9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="92">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -307,6 +308,15 @@
   </si>
   <si>
     <t>V38</t>
+  </si>
+  <si>
+    <t>V39</t>
+  </si>
+  <si>
+    <t>27.03 - 02.04.2020</t>
+  </si>
+  <si>
+    <t>V40</t>
   </si>
 </sst>
 </file>
@@ -341,7 +351,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -659,11 +669,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -711,6 +747,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1111,68 +1149,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="45">
         <v>43864</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1457,13 +1495,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>410</v>
@@ -1517,68 +1555,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="45">
         <v>43871</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1938,13 +1976,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1095</v>
@@ -1995,68 +2033,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="45">
         <v>43878</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2319,13 +2357,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>400</v>
@@ -2376,68 +2414,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="45">
         <v>43888</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2783,13 +2821,13 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="30">
         <f>SUM(F7:F19)</f>
         <v>1165</v>
@@ -2833,42 +2871,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="43">
+      <c r="G1" s="45">
         <v>43895</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -3229,13 +3267,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1010</v>
@@ -3278,42 +3316,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="43">
+      <c r="G1" s="45">
         <v>43902</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -3676,13 +3714,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1090</v>
@@ -3725,42 +3763,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="43">
+      <c r="G1" s="45">
         <v>43909</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4034,13 +4072,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>555</v>
@@ -4066,12 +4104,12 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CA3D4A-EC4E-4EB5-A47F-751E9C58F477}">
   <sheetPr>
-    <tabColor rgb="FF92D050"/>
+    <tabColor rgb="FFFF7C80"/>
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4082,42 +4120,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4321,43 +4359,81 @@
       <c r="C10" s="8">
         <v>0.875</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="20"/>
+      <c r="D10" s="8">
+        <v>0.96875</v>
+      </c>
+      <c r="E10" s="6">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5">
+        <v>120</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H10" s="6" t="s">
         <v>88</v>
       </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="10"/>
+      <c r="J10" s="10">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="7">
+        <v>43916</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="F11" s="5">
+        <v>110</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>9</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="B12" s="7">
+        <v>43917</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.24305555555555555</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="6"/>
+      <c r="F12" s="5">
+        <v>50</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="10">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
@@ -4368,7 +4444,9 @@
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
@@ -4416,16 +4494,318 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>655</v>
+        <v>935</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F8FA99-FE95-4BFC-A432-E392EC4B520A}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
+    </row>
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18">
+        <v>43918</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="30">
+        <f>SUM(F4:F16)</f>
+        <v>0</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V40, 41 valmis, lõpuks sain vigadeta testida, kodu testida arv ei klapi ikkagi.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5C75F1-C874-4FD2-818B-961F7E05A1D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFC3701-9D8A-4078-AEB4-DB22A6C2E22A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1620" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="93">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>V40</t>
+  </si>
+  <si>
+    <t>V40, 41</t>
   </si>
 </sst>
 </file>
@@ -4531,7 +4534,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4601,7 +4604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -4615,8 +4618,12 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="31"/>
+      <c r="F4" s="21">
+        <v>80</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="6" t="s">
         <v>89</v>
       </c>
@@ -4625,7 +4632,7 @@
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -4633,53 +4640,95 @@
       <c r="C5" s="8">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8">
+        <v>0.625</v>
+      </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="5">
+        <v>30</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>27</v>
+      </c>
       <c r="H5" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="7">
+        <v>43919</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E6" s="6">
+        <v>15</v>
+      </c>
+      <c r="F6" s="5">
+        <v>30</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="I6" s="6"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="C7" s="8">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="E7" s="6">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5">
+        <v>180</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>5</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8">
+        <v>0.875</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="31" t="s">
+        <v>27</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
@@ -4693,7 +4742,9 @@
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="31" t="s">
+        <v>27</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -4805,7 +4856,7 @@
       <c r="E17" s="37"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V43, lisatud Blazer, parandatud Menüüde vead
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFC3701-9D8A-4078-AEB4-DB22A6C2E22A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C7378-5A74-4E0E-A831-2358AB1B138B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1620" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1635" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="95">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>V40, 41</t>
+  </si>
+  <si>
+    <t>V42</t>
+  </si>
+  <si>
+    <t>V43, vead</t>
   </si>
 </sst>
 </file>
@@ -4534,7 +4540,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4604,7 +4610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -4632,7 +4638,7 @@
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -4647,7 +4653,7 @@
       <c r="F5" s="5">
         <v>30</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -4657,7 +4663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -4676,7 +4682,7 @@
       <c r="F6" s="5">
         <v>30</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -4687,7 +4693,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -4704,7 +4710,7 @@
       <c r="F7" s="5">
         <v>180</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -4715,7 +4721,7 @@
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -4723,30 +4729,50 @@
       <c r="C8" s="8">
         <v>0.875</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="31" t="s">
+      <c r="F8" s="5">
+        <v>120</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="7">
+        <v>43920</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="31" t="s">
+      <c r="F9" s="5">
+        <v>75</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -4856,7 +4882,7 @@
       <c r="E17" s="37"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>320</v>
+        <v>515</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V43, vidage parandused terves koodus, testide puudumised, DropDownbMenu parandamine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C7378-5A74-4E0E-A831-2358AB1B138B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979029C-56C6-4C62-AA61-AE0945D69D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1635" windowWidth="21600" windowHeight="12675" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="21600" windowHeight="12360" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="97">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>V43, vead</t>
+  </si>
+  <si>
+    <t>vigade parandused</t>
+  </si>
+  <si>
+    <t>V45</t>
   </si>
 </sst>
 </file>
@@ -4540,7 +4546,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4780,12 +4786,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="C10" s="8">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.99305555555555547</v>
+      </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="F10" s="5">
+        <v>65</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -4793,13 +4809,21 @@
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="7">
+        <v>43922</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -4882,7 +4906,7 @@
       <c r="E17" s="37"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>515</v>
+        <v>580</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V45, 46, Data testitud, CommonTermData, UnitTermData ja MeasureTermData valmis
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979029C-56C6-4C62-AA61-AE0945D69D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21452211-5E04-4B7A-9C7D-33ECD3FA076A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="21600" windowHeight="12360" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="97">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -331,7 +331,7 @@
     <t>vigade parandused</t>
   </si>
   <si>
-    <t>V45</t>
+    <t>V45, 46</t>
   </si>
 </sst>
 </file>
@@ -4546,12 +4546,13 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4802,7 +4803,9 @@
       <c r="H10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -4815,7 +4818,9 @@
       <c r="C11" s="8">
         <v>0.89583333333333337</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
       <c r="G11" s="6" t="s">
@@ -4824,7 +4829,9 @@
       <c r="H11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4832,7 +4839,9 @@
         <v>9</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>

</xml_diff>

<commit_message>
V48, 302 testi läbitud, Fasaadi testid tehtud.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C4B8C8-A8F9-4AD9-A89C-017DACE64C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C2C4F-B816-4D9D-B361-BA22309BF96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
     <sheet name="Nädal 9" sheetId="9" r:id="rId9"/>
+    <sheet name="Nädal 10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="103">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -335,6 +336,21 @@
   </si>
   <si>
     <t>V47</t>
+  </si>
+  <si>
+    <t>V48</t>
+  </si>
+  <si>
+    <t>03.04.2020 - 09.04.2020</t>
+  </si>
+  <si>
+    <t>kontrolltöö</t>
+  </si>
+  <si>
+    <t>KT, tulemus 9,5/10</t>
+  </si>
+  <si>
+    <t>V48, 49</t>
   </si>
 </sst>
 </file>
@@ -778,6 +794,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -835,7 +852,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,68 +1195,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="44" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="46">
         <v>43864</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1525,13 +1541,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>410</v>
@@ -1553,6 +1569,319 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4334FA79-598C-45D5-80FF-3ABDE694C74B}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
+    </row>
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18">
+        <v>43925</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21">
+        <v>60</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8">
+        <v>0.90625</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="30">
+        <f>SUM(F4:F16)</f>
+        <v>60</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A17:E17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1585,68 +1914,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="44" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="46">
         <v>43871</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2006,13 +2335,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1095</v>
@@ -2063,68 +2392,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="44" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="46">
         <v>43878</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2387,13 +2716,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>400</v>
@@ -2444,68 +2773,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="44" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="46">
         <v>43888</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="49"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2851,13 +3180,13 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="30">
         <f>SUM(F7:F19)</f>
         <v>1165</v>
@@ -2901,42 +3230,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="45">
+      <c r="G1" s="46">
         <v>43895</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -3297,13 +3626,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1010</v>
@@ -3346,42 +3675,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="45">
+      <c r="G1" s="46">
         <v>43902</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -3744,13 +4073,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1090</v>
@@ -3793,42 +4122,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="45">
+      <c r="G1" s="46">
         <v>43909</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4102,13 +4431,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>555</v>
@@ -4150,42 +4479,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4524,13 +4853,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>935</v>
@@ -4556,12 +4885,12 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F8FA99-FE95-4BFC-A432-E392EC4B520A}">
   <sheetPr>
-    <tabColor rgb="FF92D050"/>
+    <tabColor rgb="FFFF7C80"/>
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4571,42 +4900,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4869,7 +5198,7 @@
       <c r="G12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="52" t="s">
+      <c r="H12" s="33" t="s">
         <v>97</v>
       </c>
       <c r="I12" s="6" t="s">
@@ -4881,13 +5210,25 @@
       <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="7">
+        <v>43924</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="F13" s="5">
+        <v>140</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -4934,16 +5275,16 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>720</v>
+        <v>860</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V49 lõpuni, Infra Base Repository tests. NB! GetTest läheb läbi ilma counterBefore muutujat.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C2C4F-B816-4D9D-B361-BA22309BF96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5636861F-C9FA-4D37-8CA2-F62A99F92A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="21600" windowHeight="12360" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="108">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>V48, 49</t>
+  </si>
+  <si>
+    <t>200-250 minutit</t>
+  </si>
+  <si>
+    <t>100-200 minutit</t>
+  </si>
+  <si>
+    <t>&lt;100 minutit</t>
+  </si>
+  <si>
+    <t>Iga päev:</t>
+  </si>
+  <si>
+    <t>V49 lõpuni</t>
   </si>
 </sst>
 </file>
@@ -360,7 +375,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,16 +391,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -740,11 +787,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -852,8 +925,23 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1577,10 +1665,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,9 +1678,10 @@
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="4.85546875" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
@@ -1612,7 +1701,7 @@
       <c r="I1" s="46"/>
       <c r="J1" s="47"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48"/>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -1624,7 +1713,7 @@
       <c r="I2" s="49"/>
       <c r="J2" s="50"/>
     </row>
-    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
@@ -1653,8 +1742,11 @@
       <c r="J3" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>1</v>
       </c>
@@ -1668,7 +1760,7 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E4" s="20"/>
-      <c r="F4" s="21">
+      <c r="F4" s="53">
         <v>60</v>
       </c>
       <c r="G4" s="31" t="s">
@@ -1681,45 +1773,72 @@
         <v>17</v>
       </c>
       <c r="J4" s="22"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8">
+      <c r="B5" s="24"/>
+      <c r="C5" s="25">
         <v>0.90625</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
+      <c r="D5" s="25">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="59">
+        <v>165</v>
+      </c>
+      <c r="G5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="63"/>
+      <c r="J5" s="27"/>
+      <c r="L5" s="55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="60">
+        <v>43926</v>
+      </c>
+      <c r="C6" s="61">
+        <v>0.4375</v>
+      </c>
+      <c r="D6" s="61">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="58">
+        <v>60</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="62"/>
+      <c r="L6" s="56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
@@ -1729,11 +1848,10 @@
       <c r="I7" s="6"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
@@ -1743,11 +1861,10 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
@@ -1757,7 +1874,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -1771,11 +1888,10 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
@@ -1785,11 +1901,10 @@
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
-      <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
@@ -1799,11 +1914,13 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="7">
+        <v>43927</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
@@ -1813,11 +1930,13 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7">
+        <v>43928</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
@@ -1827,11 +1946,13 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="7">
+        <v>43929</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="6"/>
@@ -1841,11 +1962,13 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>13</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="7">
+        <v>43930</v>
+      </c>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -1865,7 +1988,7 @@
       <c r="E17" s="38"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>60</v>
+        <v>285</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -1874,12 +1997,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V51, Infra PaginatedRepository testid, HasPrevoiusPage testis on mingi viga, vahest läheb läbi, vahest mitte. Kontrollin pärast.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5636861F-C9FA-4D37-8CA2-F62A99F92A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D4D806-2A4E-4B33-968E-B2EA4739AEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="21600" windowHeight="12360" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="165" windowWidth="21600" windowHeight="12360" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="114">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -356,9 +356,6 @@
     <t>200-250 minutit</t>
   </si>
   <si>
-    <t>100-200 minutit</t>
-  </si>
-  <si>
     <t>&lt;100 minutit</t>
   </si>
   <si>
@@ -366,6 +363,27 @@
   </si>
   <si>
     <t>V49 lõpuni</t>
+  </si>
+  <si>
+    <t>code, video</t>
+  </si>
+  <si>
+    <t>html frame katsetamine, V50</t>
+  </si>
+  <si>
+    <t>projekt</t>
+  </si>
+  <si>
+    <t>esmased ideed</t>
+  </si>
+  <si>
+    <t>arutamine, õppejõudele kiri</t>
+  </si>
+  <si>
+    <t>V50</t>
+  </si>
+  <si>
+    <t>100-199 minutit</t>
   </si>
 </sst>
 </file>
@@ -817,7 +835,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -868,6 +886,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -925,19 +957,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1283,68 +1303,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="58">
         <v>43864</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1629,13 +1649,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>410</v>
@@ -1668,56 +1688,56 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
     <col min="9" max="9" width="4.85546875" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" customWidth="1"/>
     <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -1742,8 +1762,8 @@
       <c r="J3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="57" t="s">
-        <v>106</v>
+      <c r="L3" s="38" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1760,7 +1780,7 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E4" s="20"/>
-      <c r="F4" s="53">
+      <c r="F4" s="34">
         <v>60</v>
       </c>
       <c r="G4" s="31" t="s">
@@ -1773,7 +1793,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="22"/>
-      <c r="L4" s="54" t="s">
+      <c r="L4" s="35" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1789,122 +1809,181 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="59">
+      <c r="F5" s="40">
         <v>165</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>27</v>
+      <c r="G5" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="63"/>
+      <c r="I5" s="44"/>
       <c r="J5" s="27"/>
-      <c r="L5" s="55" t="s">
-        <v>104</v>
+      <c r="L5" s="36" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="41">
         <v>43926</v>
       </c>
-      <c r="C6" s="61">
+      <c r="C6" s="42">
         <v>0.4375</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="42">
         <v>0.47916666666666669</v>
       </c>
       <c r="E6" s="32"/>
-      <c r="F6" s="58">
+      <c r="F6" s="45">
         <v>60</v>
       </c>
-      <c r="G6" s="32" t="s">
-        <v>27</v>
+      <c r="G6" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="62"/>
-      <c r="L6" s="56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="43"/>
+      <c r="L6" s="37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="10"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="25">
+        <v>0.9375</v>
+      </c>
+      <c r="D7" s="25">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="40">
+        <v>140</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="10"/>
+      <c r="B8" s="7">
+        <v>43927</v>
+      </c>
+      <c r="C8" s="42">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D8" s="42">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="45">
+        <v>30</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="F9" s="65">
+        <v>60</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="10"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D10" s="25">
+        <v>0</v>
+      </c>
+      <c r="E10" s="26">
+        <v>10</v>
+      </c>
+      <c r="F10" s="40">
+        <v>110</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="10"/>
+      <c r="B11" s="7">
+        <v>43928</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
@@ -1918,9 +1997,6 @@
       <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="7">
-        <v>43927</v>
-      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
@@ -1934,9 +2010,6 @@
       <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" s="7">
-        <v>43928</v>
-      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
@@ -1979,16 +2052,16 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>285</v>
+        <v>625</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -2037,68 +2110,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="58">
         <v>43871</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2458,13 +2531,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1095</v>
@@ -2515,68 +2588,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="58">
         <v>43878</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2839,13 +2912,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>400</v>
@@ -2896,68 +2969,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="58">
         <v>43888</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3303,13 +3376,13 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="50"/>
       <c r="F20" s="30">
         <f>SUM(F7:F19)</f>
         <v>1165</v>
@@ -3353,42 +3426,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46">
+      <c r="G1" s="58">
         <v>43895</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -3749,13 +3822,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1010</v>
@@ -3798,42 +3871,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46">
+      <c r="G1" s="58">
         <v>43902</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4196,13 +4269,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1090</v>
@@ -4245,42 +4318,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46">
+      <c r="G1" s="58">
         <v>43909</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4554,13 +4627,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>555</v>
@@ -4602,42 +4675,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4976,13 +5049,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>935</v>
@@ -5023,42 +5096,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5398,13 +5471,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="50"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>860</v>

</xml_diff>

<commit_message>
V52, MeasuresRepository testid, 301 läbitud, 2 mitte
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D4D806-2A4E-4B33-968E-B2EA4739AEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670DAC0D-81D8-413A-8139-DE3A33B98B83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="165" windowWidth="21600" windowHeight="12360" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="115">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -380,10 +380,13 @@
     <t>arutamine, õppejõudele kiri</t>
   </si>
   <si>
-    <t>V50</t>
-  </si>
-  <si>
     <t>100-199 minutit</t>
+  </si>
+  <si>
+    <t>V50, 51</t>
+  </si>
+  <si>
+    <t>V52</t>
   </si>
 </sst>
 </file>
@@ -835,7 +838,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -900,6 +903,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -957,7 +966,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1303,68 +1311,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="64">
         <v>43864</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1649,13 +1657,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="50"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>410</v>
@@ -1688,7 +1696,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,42 +1710,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -1821,7 +1829,7 @@
       <c r="I5" s="44"/>
       <c r="J5" s="27"/>
       <c r="L5" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1921,7 +1929,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="65">
+      <c r="F9" s="46">
         <v>60</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -1956,48 +1964,62 @@
         <v>107</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I10" s="26" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="27"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="47">
         <v>43928</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="43"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="10"/>
+      <c r="B12" s="7">
+        <v>43929</v>
+      </c>
+      <c r="C12" s="42">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="D12" s="42">
+        <v>0.9375</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="39">
+        <v>105</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="43"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8">
+        <v>0.9375</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
@@ -2023,9 +2045,6 @@
       <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="B15" s="7">
-        <v>43929</v>
-      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="6"/>
@@ -2052,16 +2071,16 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>625</v>
+        <v>730</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -2110,68 +2129,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="64">
         <v>43871</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2531,13 +2550,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="50"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1095</v>
@@ -2588,68 +2607,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="64">
         <v>43878</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2912,13 +2931,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="50"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>400</v>
@@ -2969,68 +2988,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="57" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="64">
         <v>43888</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3376,13 +3395,13 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
       <c r="F20" s="30">
         <f>SUM(F7:F19)</f>
         <v>1165</v>
@@ -3426,42 +3445,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="58">
+      <c r="G1" s="64">
         <v>43895</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -3822,13 +3841,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1010</v>
@@ -3871,42 +3890,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="58">
+      <c r="G1" s="64">
         <v>43902</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4269,13 +4288,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1090</v>
@@ -4318,42 +4337,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="58">
+      <c r="G1" s="64">
         <v>43909</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4627,13 +4646,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>555</v>
@@ -4675,42 +4694,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5049,13 +5068,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>935</v>
@@ -5096,42 +5115,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5471,13 +5490,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>860</v>

</xml_diff>

<commit_message>
V53 tehtud, V54 enne DB kustutamist comittin töötava koodi
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670DAC0D-81D8-413A-8139-DE3A33B98B83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7FF893-0711-4360-AD27-6FBB3BB43FE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="116">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>V52</t>
+  </si>
+  <si>
+    <t>V53</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1699,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2007,9 @@
       <c r="F12" s="39">
         <v>105</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="32" t="s">
+        <v>107</v>
+      </c>
       <c r="H12" s="33" t="s">
         <v>114</v>
       </c>
@@ -2020,12 +2025,22 @@
       <c r="C13" s="8">
         <v>0.9375</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="F13" s="5">
+        <v>75</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2080,7 +2095,7 @@
       <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>730</v>
+        <v>805</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V54, lisatud migratrioonid, lisatud Aids kausta Unitsid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7FF893-0711-4360-AD27-6FBB3BB43FE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C707E69F-E1B1-4EAF-8A3E-40D995F3B2AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="117">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>V53</t>
+  </si>
+  <si>
+    <t>v54</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -835,13 +838,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -969,6 +985,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1699,7 +1717,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,34 +2012,35 @@
       <c r="A12" s="9">
         <v>9</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="18">
         <v>43929</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="19">
         <v>0.86458333333333337</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="19">
         <v>0.9375</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="39">
+      <c r="E12" s="20"/>
+      <c r="F12" s="34">
         <v>105</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="I12" s="32" t="s">
+      <c r="I12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="43"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
+      <c r="B13" s="6"/>
       <c r="C13" s="8">
         <v>0.9375</v>
       </c>
@@ -2029,7 +2048,7 @@
         <v>0.98958333333333337</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5">
+      <c r="F13" s="46">
         <v>75</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -2043,31 +2062,44 @@
       </c>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="10"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="25">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="D14" s="25">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="40">
+        <v>30</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="10"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="43"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
@@ -2095,7 +2127,7 @@
       <c r="E17" s="56"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
-        <v>805</v>
+        <v>835</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>

<commit_message>
V55 units repo testid tehtud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C707E69F-E1B1-4EAF-8A3E-40D995F3B2AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F9CCF3-0B69-40C0-B2A3-1915908D99CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="119">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>v54</t>
+  </si>
+  <si>
+    <t>TDD, XP, K.Beck</t>
+  </si>
+  <si>
+    <t>V54</t>
   </si>
 </sst>
 </file>
@@ -459,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -851,13 +857,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -915,7 +932,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -928,6 +944,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -985,8 +1005,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1332,68 +1350,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="67">
         <v>43864</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1678,13 +1696,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>410</v>
@@ -1714,10 +1732,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F15" sqref="F15:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,42 +1749,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -1838,7 +1856,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="40">
+      <c r="F5" s="39">
         <v>165</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -1847,7 +1865,7 @@
       <c r="H5" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="44"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="27"/>
       <c r="L5" s="36" t="s">
         <v>112</v>
@@ -1857,17 +1875,17 @@
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="40">
         <v>43926</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="41">
         <v>0.4375</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="41">
         <v>0.47916666666666669</v>
       </c>
       <c r="E6" s="32"/>
-      <c r="F6" s="45">
+      <c r="F6" s="44">
         <v>60</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -1879,7 +1897,7 @@
       <c r="I6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="43"/>
+      <c r="J6" s="42"/>
       <c r="L6" s="37" t="s">
         <v>104</v>
       </c>
@@ -1896,7 +1914,7 @@
         <v>3.4722222222222224E-2</v>
       </c>
       <c r="E7" s="26"/>
-      <c r="F7" s="40">
+      <c r="F7" s="39">
         <v>140</v>
       </c>
       <c r="G7" s="26" t="s">
@@ -1917,14 +1935,14 @@
       <c r="B8" s="7">
         <v>43927</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="41">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="41">
         <v>0.60416666666666663</v>
       </c>
       <c r="E8" s="32"/>
-      <c r="F8" s="45">
+      <c r="F8" s="44">
         <v>30</v>
       </c>
       <c r="G8" s="32" t="s">
@@ -1936,7 +1954,7 @@
       <c r="I8" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -1950,7 +1968,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="46">
+      <c r="F9" s="45">
         <v>60</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -1978,7 +1996,7 @@
       <c r="E10" s="26">
         <v>10</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="39">
         <v>110</v>
       </c>
       <c r="G10" s="26" t="s">
@@ -1996,17 +2014,17 @@
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="46">
         <v>43928</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="51"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="50"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -2028,7 +2046,7 @@
       <c r="G12" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="51" t="s">
         <v>114</v>
       </c>
       <c r="I12" s="20" t="s">
@@ -2048,7 +2066,7 @@
         <v>0.98958333333333337</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="46">
+      <c r="F13" s="45">
         <v>75</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -2066,7 +2084,7 @@
       <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" s="72"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="25">
         <v>0.98958333333333337</v>
       </c>
@@ -2074,7 +2092,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E14" s="26"/>
-      <c r="F14" s="40">
+      <c r="F14" s="39">
         <v>30</v>
       </c>
       <c r="G14" s="26" t="s">
@@ -2092,51 +2110,94 @@
       <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
+      <c r="B15" s="7">
+        <v>43930</v>
+      </c>
+      <c r="C15" s="41">
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="D15" s="41">
+        <v>0.2986111111111111</v>
+      </c>
       <c r="E15" s="32"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
+      <c r="F15" s="44">
+        <v>60</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>117</v>
+      </c>
       <c r="I15" s="32"/>
-      <c r="J15" s="43"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="42"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
-      <c r="B16" s="7">
-        <v>43930</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="32"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="41">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="D16" s="41">
+        <v>0.9375</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="44">
+        <v>40</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>109</v>
+      </c>
       <c r="H16" s="32"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="41">
+        <v>0.9375</v>
+      </c>
+      <c r="D17" s="41">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="44">
+        <v>105</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="30">
-        <f>SUM(F4:F16)</f>
-        <v>835</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="29"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="30">
+        <f>SUM(F4:F17)</f>
+        <v>1040</v>
+      </c>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:J1"/>
@@ -2176,68 +2237,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="67">
         <v>43871</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2597,13 +2658,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1095</v>
@@ -2654,68 +2715,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="67">
         <v>43878</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2978,13 +3039,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>400</v>
@@ -3035,68 +3096,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="67">
         <v>43888</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3442,13 +3503,13 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
       <c r="F20" s="30">
         <f>SUM(F7:F19)</f>
         <v>1165</v>
@@ -3492,42 +3553,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="64">
+      <c r="G1" s="67">
         <v>43895</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -3888,13 +3949,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1010</v>
@@ -3937,42 +3998,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="64">
+      <c r="G1" s="67">
         <v>43902</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4335,13 +4396,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1090</v>
@@ -4384,42 +4445,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="64">
+      <c r="G1" s="67">
         <v>43909</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4693,13 +4754,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>555</v>
@@ -4741,42 +4802,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5115,13 +5176,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>935</v>
@@ -5162,42 +5223,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5537,13 +5598,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>860</v>

</xml_diff>

<commit_message>
V56, Test Infrasse on lisatud teised Repositoryd, 1 test ei lähe läbi (UpdateTest)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F9CCF3-0B69-40C0-B2A3-1915908D99CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1B111-41F6-4B16-A606-34F01CBD34EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="12735" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
     <sheet name="Nädal 9" sheetId="9" r:id="rId9"/>
     <sheet name="Nädal 10" sheetId="10" r:id="rId10"/>
+    <sheet name="Nädal 11" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="121">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -399,6 +400,12 @@
   </si>
   <si>
     <t>V54</t>
+  </si>
+  <si>
+    <t>video, code</t>
+  </si>
+  <si>
+    <t>V56</t>
   </si>
 </sst>
 </file>
@@ -465,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -868,13 +875,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1005,6 +1049,37 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1730,12 +1805,12 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4334FA79-598C-45D5-80FF-3ABDE694C74B}">
   <sheetPr>
-    <tabColor rgb="FF92D050"/>
+    <tabColor rgb="FFFF7C80"/>
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,6 +2278,332 @@
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A735C472-1494-4C33-B9A6-4F10FA99B28A}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
+    </row>
+    <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="84">
+        <v>43931</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.59375</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="L4" s="35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="L5" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="L6" s="37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="81">
+        <f>SUM(F4:F17)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="83"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V57, Infra Quantity repo testid, UnitFactors, UnitTerms
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1B111-41F6-4B16-A606-34F01CBD34EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F473D5FC-A746-4FC6-BF7E-5E274ED1CCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="12735" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="122">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>V56</t>
+  </si>
+  <si>
+    <t>V57</t>
   </si>
 </sst>
 </file>
@@ -992,6 +995,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1049,37 +1074,15 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1425,68 +1428,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="65"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="66" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="67">
+      <c r="G4" s="75">
         <v>43864</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="79"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="56"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -1771,13 +1774,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>410</v>
@@ -1824,42 +1827,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -2254,13 +2257,13 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="59"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="30">
         <f>SUM(F4:F17)</f>
         <v>1040</v>
@@ -2291,7 +2294,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,64 +2305,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="75" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="78" t="s">
+      <c r="J3" s="58" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="38" t="s">
@@ -2367,25 +2370,31 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="37">
         <v>1</v>
       </c>
-      <c r="B4" s="84">
+      <c r="B4" s="62">
         <v>43931</v>
       </c>
       <c r="C4" s="8">
         <v>0.59375</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="8">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6">
+        <v>75</v>
+      </c>
       <c r="G4" s="6" t="s">
         <v>119</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J4" s="6"/>
       <c r="L4" s="35" t="s">
         <v>103</v>
@@ -2395,14 +2404,28 @@
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="62">
+        <v>43932</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="F5" s="6">
+        <v>55</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="L5" s="36" t="s">
         <v>112</v>
@@ -2580,30 +2603,30 @@
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="81">
+      <c r="B18" s="82"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="59">
         <f>SUM(F4:F17)</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="83"/>
+        <v>130</v>
+      </c>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A18:E18"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2638,68 +2661,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="65"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="66" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="67">
+      <c r="G4" s="75">
         <v>43871</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="79"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="56"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3059,13 +3082,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1095</v>
@@ -3116,68 +3139,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="65"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="66" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="67">
+      <c r="G4" s="75">
         <v>43878</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="79"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="56"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3440,13 +3463,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>400</v>
@@ -3497,68 +3520,68 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="65"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="66" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="67">
+      <c r="G4" s="75">
         <v>43888</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="79"/>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="56"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3904,13 +3927,13 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="30">
         <f>SUM(F7:F19)</f>
         <v>1165</v>
@@ -3954,42 +3977,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="67">
+      <c r="G1" s="75">
         <v>43895</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4350,13 +4373,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1010</v>
@@ -4399,42 +4422,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="67">
+      <c r="G1" s="75">
         <v>43902</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -4797,13 +4820,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>1090</v>
@@ -4846,42 +4869,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="67">
+      <c r="G1" s="75">
         <v>43909</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5155,13 +5178,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>555</v>
@@ -5203,42 +5226,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5577,13 +5600,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>935</v>
@@ -5624,42 +5647,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5999,13 +6022,13 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="30">
         <f>SUM(F4:F16)</f>
         <v>860</v>

</xml_diff>